<commit_message>
v1.2 update owner status
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_PUBLISHARTICLE_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_PUBLISHARTICLE_REVIEWS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="LH_WF_PUBLISHARTICLE_REVIEW" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -104,12 +104,15 @@
   </si>
   <si>
     <t>add an example of invalid article error messages in the SRS like "article body exceeds 1000 words"</t>
+  </si>
+  <si>
+    <t>closed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -322,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -407,9 +410,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,7 +471,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -506,7 +506,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -683,7 +683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -763,7 +763,7 @@
         <v>18</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I2" s="17" t="s">
         <v>15</v>
@@ -791,8 +791,8 @@
       <c r="G3" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="29" t="s">
-        <v>15</v>
+      <c r="H3" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="I3" s="20" t="s">
         <v>15</v>
@@ -821,7 +821,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="I4" s="17" t="s">
         <v>15</v>
@@ -933,7 +933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v1.1 verify that the previous comments modified
close publish article wireframe review and verify the updates
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_WF_PUBLISHARTICLE_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_WF_PUBLISHARTICLE_REVIEWS.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
@@ -10,7 +10,7 @@
     <sheet name="LH_WF_PUBLISHARTICLE_REVIEW" sheetId="3" r:id="rId1"/>
     <sheet name="VERSION-HISTORY" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Ahmed Abuzaid</t>
   </si>
   <si>
-    <t>open</t>
-  </si>
-  <si>
     <t>28/4/2025</t>
   </si>
   <si>
@@ -107,12 +104,18 @@
   </si>
   <si>
     <t>closed</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">close the review status </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -325,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -410,6 +413,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -683,7 +689,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -694,7 +700,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -742,10 +748,10 @@
     </row>
     <row r="2" spans="1:9" ht="90">
       <c r="A2" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>17</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>14</v>
@@ -754,27 +760,27 @@
         <v>13</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="60">
       <c r="A3" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>14</v>
@@ -783,27 +789,27 @@
         <v>13</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>28</v>
+        <v>17</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>27</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="75">
       <c r="A4" s="28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>14</v>
@@ -812,19 +818,19 @@
         <v>13</v>
       </c>
       <c r="E4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="G4" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>28</v>
-      </c>
       <c r="I4" s="17" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -934,7 +940,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -967,17 +973,25 @@
         <v>14</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="10">
         <v>45775</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="10">
+        <v>45776</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="18.75">
       <c r="A4" s="8"/>

</xml_diff>